<commit_message>
add MIAPPE example values
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIAPPE/MIAPPE_-_Experimental_factors.xlsx
+++ b/templates/dataplant/MIAPPE/MIAPPE_-_Experimental_factors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -393,6 +393,84 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>spring season</t>
+  </si>
+  <si>
+    <t>ENVO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ENVO_00000027</t>
+  </si>
+  <si>
+    <t>28/25°C (Day/Night)</t>
+  </si>
+  <si>
+    <t>27/25°C (Day/Night)</t>
+  </si>
+  <si>
+    <t>sand content (10 % v/v)</t>
+  </si>
+  <si>
+    <t>actinomycin D; 20mM;20ml per plant; Every week</t>
+  </si>
+  <si>
+    <t>Bion; 13,5mM; 5ml per plant; Every 15 days.</t>
+  </si>
+  <si>
+    <t>rice tungro bacilliform virus (RTBV) 2.5 µl, incubated at room temperature for 10min</t>
+  </si>
+  <si>
+    <t>Potassium phosphate; 50 Kg P.Ha/y 50 Kg K.Ha/y</t>
+  </si>
+  <si>
+    <t>Benzothiadiazole; 10mM; 1ml; Every month</t>
+  </si>
+  <si>
+    <t>Carbon Dioxide; 20ppm</t>
+  </si>
+  <si>
+    <t>Zero gravity (International space station)</t>
+  </si>
+  <si>
+    <t>Jasmonic acid; 1mM;20ml</t>
+  </si>
+  <si>
+    <t>SUREWET (Polyvinyl polymer and nonionic surfactant); 1,75mM; 5ml per plant; Sprayed every month</t>
+  </si>
+  <si>
+    <t>wounding</t>
+  </si>
+  <si>
+    <t>Cd 0.5 mg/L (Hydroponics)</t>
+  </si>
+  <si>
+    <t>56%/70% (Day/Night)</t>
+  </si>
+  <si>
+    <t>200-280nm; 30min; every day</t>
+  </si>
+  <si>
+    <t>79 rainfall events; 15,6mm (mean size)</t>
+  </si>
+  <si>
+    <t>NaCl:150mM ; KCl:30mM</t>
+  </si>
+  <si>
+    <t>20ml every 3 days</t>
+  </si>
+  <si>
+    <t>20°C</t>
+  </si>
+  <si>
+    <t>Flooding water</t>
+  </si>
+  <si>
+    <t>Glyphosfate; 1.68 kg acid equivalent (a.e.) / ha</t>
+  </si>
+  <si>
+    <t>acidic pH soil environment</t>
   </si>
 </sst>
 </file>
@@ -1370,16 +1448,16 @@
         <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
         <v>126</v>
@@ -1388,7 +1466,7 @@
         <v>126</v>
       </c>
       <c r="H2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
         <v>126</v>
@@ -1397,7 +1475,7 @@
         <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="L2" t="s">
         <v>126</v>
@@ -1406,7 +1484,7 @@
         <v>126</v>
       </c>
       <c r="N2" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="O2" t="s">
         <v>126</v>
@@ -1415,7 +1493,7 @@
         <v>126</v>
       </c>
       <c r="Q2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="R2" t="s">
         <v>126</v>
@@ -1424,7 +1502,7 @@
         <v>126</v>
       </c>
       <c r="T2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="U2" t="s">
         <v>126</v>
@@ -1433,7 +1511,7 @@
         <v>126</v>
       </c>
       <c r="W2" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="X2" t="s">
         <v>126</v>
@@ -1442,7 +1520,7 @@
         <v>126</v>
       </c>
       <c r="Z2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="AA2" t="s">
         <v>126</v>
@@ -1451,7 +1529,7 @@
         <v>126</v>
       </c>
       <c r="AC2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="AD2" t="s">
         <v>126</v>
@@ -1460,7 +1538,7 @@
         <v>126</v>
       </c>
       <c r="AF2" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="AG2" t="s">
         <v>126</v>
@@ -1469,7 +1547,7 @@
         <v>126</v>
       </c>
       <c r="AI2" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="AJ2" t="s">
         <v>126</v>
@@ -1478,7 +1556,7 @@
         <v>126</v>
       </c>
       <c r="AL2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="AM2" t="s">
         <v>126</v>
@@ -1487,7 +1565,7 @@
         <v>126</v>
       </c>
       <c r="AO2" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="AP2" t="s">
         <v>126</v>
@@ -1496,7 +1574,7 @@
         <v>126</v>
       </c>
       <c r="AR2" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="AS2" t="s">
         <v>126</v>
@@ -1505,7 +1583,7 @@
         <v>126</v>
       </c>
       <c r="AU2" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="AV2" t="s">
         <v>126</v>
@@ -1514,7 +1592,7 @@
         <v>126</v>
       </c>
       <c r="AX2" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="AY2" t="s">
         <v>126</v>
@@ -1523,7 +1601,7 @@
         <v>126</v>
       </c>
       <c r="BA2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="BB2" t="s">
         <v>126</v>
@@ -1532,7 +1610,7 @@
         <v>126</v>
       </c>
       <c r="BD2" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="BE2" t="s">
         <v>126</v>
@@ -1541,7 +1619,7 @@
         <v>126</v>
       </c>
       <c r="BG2" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="BH2" t="s">
         <v>126</v>
@@ -1550,7 +1628,7 @@
         <v>126</v>
       </c>
       <c r="BJ2" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="BK2" t="s">
         <v>126</v>
@@ -1559,7 +1637,7 @@
         <v>126</v>
       </c>
       <c r="BM2" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="BN2" t="s">
         <v>126</v>
@@ -1568,7 +1646,7 @@
         <v>126</v>
       </c>
       <c r="BP2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="BQ2" t="s">
         <v>126</v>
@@ -1577,7 +1655,7 @@
         <v>126</v>
       </c>
       <c r="BS2" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="BT2" t="s">
         <v>126</v>

</xml_diff>